<commit_message>
updated fis_sus_score, gap filled
</commit_message>
<xml_diff>
--- a/prep/FIS/fis_sbsbmsy.xlsx
+++ b/prep/FIS/fis_sbsbmsy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="16860" yWindow="-90" windowWidth="9555" windowHeight="6435"/>
+    <workbookView xWindow="9615" yWindow="345" windowWidth="16695" windowHeight="6435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -244,6 +243,218 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$1:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$1:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.2162037037037039</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2273550724637681</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1983091787439615</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1137681159420292</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9839371980676328</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1385869565217392</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2198470209339773</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2698671497584542</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.2915458937198068</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2510668276972625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="186568704"/>
+        <c:axId val="186525568"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="186568704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="186525568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="186525568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="186568704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>376237</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>71437</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,13 +2489,203 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>110101</v>
+      </c>
+      <c r="B1">
+        <v>49680</v>
+      </c>
+      <c r="C1">
+        <f>A1/B1</f>
+        <v>2.2162037037037039</v>
+      </c>
+      <c r="D1">
+        <v>2012</v>
+      </c>
+      <c r="E1">
+        <v>2.2162037037037039</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>110655</v>
+      </c>
+      <c r="B2">
+        <v>49680</v>
+      </c>
+      <c r="C2">
+        <f>A2/B2</f>
+        <v>2.2273550724637681</v>
+      </c>
+      <c r="D2">
+        <v>2011</v>
+      </c>
+      <c r="E2">
+        <v>2.2273550724637681</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>109212</v>
+      </c>
+      <c r="B3">
+        <v>49680</v>
+      </c>
+      <c r="C3">
+        <f>A3/B3</f>
+        <v>2.1983091787439615</v>
+      </c>
+      <c r="D3">
+        <v>2010</v>
+      </c>
+      <c r="E3">
+        <v>2.1983091787439615</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>105012</v>
+      </c>
+      <c r="B4">
+        <v>49680</v>
+      </c>
+      <c r="C4">
+        <f>A4/B4</f>
+        <v>2.1137681159420292</v>
+      </c>
+      <c r="D4">
+        <v>2009</v>
+      </c>
+      <c r="E4">
+        <v>2.1137681159420292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>98562</v>
+      </c>
+      <c r="B5">
+        <v>49680</v>
+      </c>
+      <c r="C5">
+        <f>A5/B5</f>
+        <v>1.9839371980676328</v>
+      </c>
+      <c r="D5">
+        <v>2008</v>
+      </c>
+      <c r="E5">
+        <v>1.9839371980676328</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>106245</v>
+      </c>
+      <c r="B6">
+        <v>49680</v>
+      </c>
+      <c r="C6">
+        <f>A6/B6</f>
+        <v>2.1385869565217392</v>
+      </c>
+      <c r="D6">
+        <v>2007</v>
+      </c>
+      <c r="E6">
+        <v>2.1385869565217392</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>110282</v>
+      </c>
+      <c r="B7">
+        <v>49680</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:E10" si="0">A7/B7</f>
+        <v>2.2198470209339773</v>
+      </c>
+      <c r="D7">
+        <v>2006</v>
+      </c>
+      <c r="E7">
+        <v>2.2198470209339773</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>112767</v>
+      </c>
+      <c r="B8">
+        <v>49680</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>2.2698671497584542</v>
+      </c>
+      <c r="D8">
+        <v>2005</v>
+      </c>
+      <c r="E8">
+        <v>2.2698671497584542</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>113844</v>
+      </c>
+      <c r="B9">
+        <v>49680</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>2.2915458937198068</v>
+      </c>
+      <c r="D9">
+        <v>2004</v>
+      </c>
+      <c r="E9">
+        <v>2.2915458937198068</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>111833</v>
+      </c>
+      <c r="B10">
+        <v>49680</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2.2510668276972625</v>
+      </c>
+      <c r="D10">
+        <v>2003</v>
+      </c>
+      <c r="E10">
+        <v>2.2510668276972625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f>AVERAGE(E1:E10)</f>
+        <v>2.1910487117552333</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>